<commit_message>
Updated data files with most recent
</commit_message>
<xml_diff>
--- a/data_raw/IEPFishCodes.xlsx
+++ b/data_raw/IEPFishCodes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/catarina_pien_water_ca_gov/Documents/Work/Database/DataPublication/FishPublication/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/catarina_pien_water_ca_gov/Documents/Work/Database/DataPublication/publish_fish/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{0E58D790-2FCA-4A3F-8F41-0F8B140D6F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55ABEB76-C64B-4CBA-B219-17768AC441FF}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{0E58D790-2FCA-4A3F-8F41-0F8B140D6F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4716387D-D196-4CB3-B2FD-882F99A57D9F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="227" activeTab="1" xr2:uid="{954D08CE-A2BF-49C1-8AF9-792A340A95CF}"/>
   </bookViews>
@@ -1099,9 +1099,6 @@
     <t>Sebastes mystinus</t>
   </si>
   <si>
-    <t>BLUKILL </t>
-  </si>
-  <si>
     <t>Bluefin Killifish </t>
   </si>
   <si>
@@ -3125,6 +3122,9 @@
   </si>
   <si>
     <t>STRBA3</t>
+  </si>
+  <si>
+    <t>BLUKIL</t>
   </si>
 </sst>
 </file>
@@ -4659,7 +4659,7 @@
   <sheetData>
     <row r="1" spans="1:28" s="49" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B1" s="55" t="s">
         <v>0</v>
@@ -4674,10 +4674,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="59" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="H1" s="51" t="s">
         <v>4</v>
@@ -4745,7 +4745,7 @@
     </row>
     <row r="2" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B2" s="61" t="s">
         <v>25</v>
@@ -4827,7 +4827,7 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B3" s="67" t="s">
         <v>33</v>
@@ -4871,7 +4871,7 @@
     </row>
     <row r="4" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B4" s="67" t="s">
         <v>36</v>
@@ -4915,7 +4915,7 @@
     </row>
     <row r="5" spans="1:28" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B5" s="67" t="s">
         <v>39</v>
@@ -4961,7 +4961,7 @@
     </row>
     <row r="6" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B6" s="67" t="s">
         <v>43</v>
@@ -5015,7 +5015,7 @@
     </row>
     <row r="7" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B7" s="67" t="s">
         <v>49</v>
@@ -5063,7 +5063,7 @@
     </row>
     <row r="8" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B8" s="67" t="s">
         <v>52</v>
@@ -5109,7 +5109,7 @@
     </row>
     <row r="9" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B9" s="67" t="s">
         <v>55</v>
@@ -5153,7 +5153,7 @@
     </row>
     <row r="10" spans="1:28" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B10" s="67" t="s">
         <v>58</v>
@@ -5209,7 +5209,7 @@
     </row>
     <row r="11" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B11" s="67" t="s">
         <v>61</v>
@@ -5257,7 +5257,7 @@
     </row>
     <row r="12" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B12" s="67" t="s">
         <v>65</v>
@@ -5309,7 +5309,7 @@
     </row>
     <row r="13" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B13" s="67" t="s">
         <v>69</v>
@@ -6716,7 +6716,7 @@
         <v>169</v>
       </c>
       <c r="D40" s="63" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E40" s="64"/>
       <c r="F40" s="65" t="s">
@@ -6762,7 +6762,7 @@
         <v>172</v>
       </c>
       <c r="D41" s="63" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E41" s="64"/>
       <c r="F41" s="65" t="s">
@@ -6808,7 +6808,7 @@
         <v>174</v>
       </c>
       <c r="D42" s="63" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E42" s="64"/>
       <c r="F42" s="65" t="s">
@@ -7234,7 +7234,7 @@
         <v>217</v>
       </c>
       <c r="D49" s="63" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="E49" s="64"/>
       <c r="F49" s="65" t="s">
@@ -7299,7 +7299,7 @@
     </row>
     <row r="50" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B50" s="86" t="s">
         <v>221</v>
@@ -7308,7 +7308,7 @@
         <v>222</v>
       </c>
       <c r="D50" s="88" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="E50" s="64"/>
       <c r="F50" s="65"/>
@@ -7373,7 +7373,7 @@
     </row>
     <row r="51" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B51" s="86" t="s">
         <v>228</v>
@@ -7382,7 +7382,7 @@
         <v>229</v>
       </c>
       <c r="D51" s="63" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="E51" s="64"/>
       <c r="F51" s="65" t="s">
@@ -7455,7 +7455,7 @@
     </row>
     <row r="52" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B52" s="86" t="s">
         <v>232</v>
@@ -7464,7 +7464,7 @@
         <v>233</v>
       </c>
       <c r="D52" s="63" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E52" s="64"/>
       <c r="F52" s="65" t="s">
@@ -7513,7 +7513,7 @@
     </row>
     <row r="53" spans="1:29" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B53" s="93" t="s">
         <v>238</v>
@@ -7522,7 +7522,7 @@
         <v>239</v>
       </c>
       <c r="D53" s="95" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E53" s="64"/>
       <c r="F53" s="96"/>
@@ -7579,7 +7579,7 @@
     </row>
     <row r="54" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A54" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B54" s="93" t="s">
         <v>244</v>
@@ -7588,7 +7588,7 @@
         <v>245</v>
       </c>
       <c r="D54" s="95" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="E54" s="64"/>
       <c r="F54" s="96"/>
@@ -7629,7 +7629,7 @@
     </row>
     <row r="55" spans="1:29" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A55" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B55" s="93" t="s">
         <v>248</v>
@@ -7686,7 +7686,7 @@
     </row>
     <row r="56" spans="1:29" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A56" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B56" s="93" t="s">
         <v>252</v>
@@ -7753,7 +7753,7 @@
     </row>
     <row r="57" spans="1:29" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A57" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B57" s="93" t="s">
         <v>259</v>
@@ -7812,7 +7812,7 @@
     </row>
     <row r="58" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A58" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B58" s="93" t="s">
         <v>264</v>
@@ -7869,7 +7869,7 @@
     </row>
     <row r="59" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B59" s="61" t="s">
         <v>269</v>
@@ -7938,7 +7938,7 @@
     </row>
     <row r="60" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B60" s="61" t="s">
         <v>274</v>
@@ -7983,7 +7983,7 @@
     </row>
     <row r="61" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B61" s="61" t="s">
         <v>276</v>
@@ -8042,7 +8042,7 @@
     </row>
     <row r="62" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B62" s="61" t="s">
         <v>281</v>
@@ -8088,7 +8088,7 @@
     </row>
     <row r="63" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B63" s="61" t="s">
         <v>284</v>
@@ -8130,7 +8130,7 @@
     </row>
     <row r="64" spans="1:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="114" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B64" s="115" t="s">
         <v>287</v>
@@ -8184,8 +8184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BE88D6D-0F10-42CC-A619-076727350CF2}">
   <dimension ref="A1:Q1036"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8201,7 +8201,7 @@
         <v>290</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C1" s="24" t="s">
         <v>291</v>
@@ -8435,28 +8435,28 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="36" t="s">
+        <v>944</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>353</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="C18" s="27" t="s">
         <v>354</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="D18" s="15" t="s">
         <v>355</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>357</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="C19" s="17" t="s">
         <v>358</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>359</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>339</v>
@@ -8464,13 +8464,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="B20" s="25" t="s">
         <v>360</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="C20" s="17" t="s">
         <v>361</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>362</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>346</v>
@@ -8478,69 +8478,69 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>363</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="C21" s="17" t="s">
         <v>364</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="D21" s="15" t="s">
         <v>365</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
+        <v>366</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>367</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="C22" s="30" t="s">
         <v>368</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="D22" s="16" t="s">
         <v>369</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="B23" s="29" t="s">
         <v>371</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="C23" s="30" t="s">
         <v>372</v>
       </c>
-      <c r="C23" s="30" t="s">
-        <v>373</v>
-      </c>
       <c r="D23" s="28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="B24" s="29" t="s">
         <v>374</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="C24" s="31" t="s">
         <v>375</v>
       </c>
-      <c r="C24" s="31" t="s">
+      <c r="D24" s="28" t="s">
         <v>376</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="B25" s="29" t="s">
         <v>378</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="C25" s="30" t="s">
         <v>379</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>380</v>
       </c>
       <c r="D25" s="28" t="s">
         <v>335</v>
@@ -8548,13 +8548,13 @@
     </row>
     <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="B26" s="29" t="s">
         <v>381</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="C26" s="30" t="s">
         <v>382</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>383</v>
       </c>
       <c r="D26" s="28" t="s">
         <v>346</v>
@@ -8562,69 +8562,69 @@
     </row>
     <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
+        <v>383</v>
+      </c>
+      <c r="B27" s="29" t="s">
         <v>384</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="C27" s="30" t="s">
         <v>385</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="D27" s="28" t="s">
         <v>386</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
+        <v>387</v>
+      </c>
+      <c r="B28" s="29" t="s">
         <v>388</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="C28" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="C28" s="30" t="s">
-        <v>390</v>
-      </c>
       <c r="D28" s="28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="B29" s="29" t="s">
         <v>391</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="C29" s="31" t="s">
         <v>392</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="D29" s="28" t="s">
         <v>393</v>
-      </c>
-      <c r="D29" s="28" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
+        <v>394</v>
+      </c>
+      <c r="B30" s="29" t="s">
         <v>395</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="C30" s="30" t="s">
         <v>396</v>
       </c>
-      <c r="C30" s="30" t="s">
-        <v>397</v>
-      </c>
       <c r="D30" s="28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
+        <v>397</v>
+      </c>
+      <c r="B31" s="29" t="s">
         <v>398</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="C31" s="30" t="s">
         <v>399</v>
-      </c>
-      <c r="C31" s="30" t="s">
-        <v>400</v>
       </c>
       <c r="D31" s="28" t="s">
         <v>308</v>
@@ -8632,27 +8632,27 @@
     </row>
     <row r="32" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
+        <v>400</v>
+      </c>
+      <c r="B32" s="29" t="s">
         <v>401</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="C32" s="31" t="s">
         <v>402</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="D32" s="28" t="s">
         <v>403</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="B33" s="25" t="s">
         <v>405</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="C33" s="21" t="s">
         <v>406</v>
-      </c>
-      <c r="C33" s="21" t="s">
-        <v>407</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>323</v>
@@ -8660,27 +8660,27 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="B34" s="25" t="s">
         <v>408</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="C34" s="17" t="s">
         <v>409</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="D34" s="15" t="s">
         <v>410</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="B35" s="25" t="s">
         <v>412</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="C35" s="17" t="s">
         <v>413</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>414</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>327</v>
@@ -8688,41 +8688,41 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="B36" s="25" t="s">
         <v>415</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="C36" s="17" t="s">
         <v>416</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="D36" s="15" t="s">
         <v>417</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="B37" s="25" t="s">
         <v>419</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="C37" s="17" t="s">
         <v>420</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="D37" s="15" t="s">
         <v>421</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="B38" s="25" t="s">
         <v>423</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="C38" s="17" t="s">
         <v>424</v>
-      </c>
-      <c r="C38" s="17" t="s">
-        <v>425</v>
       </c>
       <c r="D38" s="15" t="s">
         <v>304</v>
@@ -8730,13 +8730,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="B39" s="25" t="s">
         <v>426</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="C39" s="17" t="s">
         <v>427</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>428</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>335</v>
@@ -8744,13 +8744,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="B40" s="25" t="s">
         <v>429</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="C40" s="17" t="s">
         <v>430</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>431</v>
       </c>
       <c r="D40" s="15" t="s">
         <v>304</v>
@@ -8758,153 +8758,153 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="B41" s="25" t="s">
         <v>432</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="C41" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>434</v>
-      </c>
       <c r="D41" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
+        <v>434</v>
+      </c>
+      <c r="B42" s="25" t="s">
         <v>435</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="C42" s="17" t="s">
         <v>436</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>437</v>
-      </c>
       <c r="D42" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
+        <v>437</v>
+      </c>
+      <c r="B43" s="25" t="s">
         <v>438</v>
       </c>
-      <c r="B43" s="25" t="s">
+      <c r="C43" s="17" t="s">
         <v>439</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>440</v>
-      </c>
       <c r="D43" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="B44" s="25" t="s">
         <v>441</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="C44" s="17" t="s">
         <v>442</v>
       </c>
-      <c r="C44" s="17" t="s">
-        <v>443</v>
-      </c>
       <c r="D44" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="B45" s="25" t="s">
         <v>444</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="C45" s="19" t="s">
         <v>445</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="D45" s="15" t="s">
         <v>446</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
+        <v>447</v>
+      </c>
+      <c r="B46" s="25" t="s">
         <v>448</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="C46" s="17" t="s">
         <v>449</v>
       </c>
-      <c r="C46" s="17" t="s">
-        <v>450</v>
-      </c>
       <c r="D46" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
+        <v>450</v>
+      </c>
+      <c r="B47" s="25" t="s">
         <v>451</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="C47" s="17" t="s">
         <v>452</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="D47" s="15" t="s">
         <v>453</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
+        <v>454</v>
+      </c>
+      <c r="B48" s="25" t="s">
         <v>455</v>
       </c>
-      <c r="B48" s="25" t="s">
+      <c r="C48" s="17" t="s">
         <v>456</v>
       </c>
-      <c r="C48" s="17" t="s">
-        <v>457</v>
-      </c>
       <c r="D48" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
+        <v>457</v>
+      </c>
+      <c r="B49" s="25" t="s">
         <v>458</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="C49" s="30" t="s">
         <v>459</v>
       </c>
-      <c r="C49" s="30" t="s">
-        <v>460</v>
-      </c>
       <c r="D49" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
+        <v>460</v>
+      </c>
+      <c r="B50" s="25" t="s">
         <v>461</v>
       </c>
-      <c r="B50" s="25" t="s">
+      <c r="C50" s="17" t="s">
         <v>462</v>
       </c>
-      <c r="C50" s="17" t="s">
-        <v>463</v>
-      </c>
       <c r="D50" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
+        <v>463</v>
+      </c>
+      <c r="B51" s="25" t="s">
         <v>464</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="C51" s="17" t="s">
         <v>465</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>466</v>
       </c>
       <c r="D51" s="15" t="s">
         <v>308</v>
@@ -8912,111 +8912,111 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="B52" s="25" t="s">
         <v>467</v>
       </c>
-      <c r="B52" s="25" t="s">
+      <c r="C52" s="17" t="s">
         <v>468</v>
       </c>
-      <c r="C52" s="17" t="s">
-        <v>469</v>
-      </c>
       <c r="D52" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
+        <v>469</v>
+      </c>
+      <c r="B53" s="25" t="s">
         <v>470</v>
       </c>
-      <c r="B53" s="25" t="s">
+      <c r="C53" s="17" t="s">
         <v>471</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>472</v>
-      </c>
       <c r="D53" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
+        <v>472</v>
+      </c>
+      <c r="B54" s="25" t="s">
         <v>473</v>
       </c>
-      <c r="B54" s="25" t="s">
+      <c r="C54" s="19" t="s">
         <v>474</v>
       </c>
-      <c r="C54" s="19" t="s">
-        <v>475</v>
-      </c>
       <c r="D54" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
+        <v>475</v>
+      </c>
+      <c r="B55" s="25" t="s">
         <v>476</v>
       </c>
-      <c r="B55" s="25" t="s">
+      <c r="C55" s="19" t="s">
         <v>477</v>
       </c>
-      <c r="C55" s="19" t="s">
-        <v>478</v>
-      </c>
       <c r="D55" s="15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
+        <v>478</v>
+      </c>
+      <c r="B56" s="25" t="s">
         <v>479</v>
       </c>
-      <c r="B56" s="25" t="s">
+      <c r="C56" s="17" t="s">
         <v>480</v>
       </c>
-      <c r="C56" s="17" t="s">
-        <v>481</v>
-      </c>
       <c r="D56" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
+        <v>481</v>
+      </c>
+      <c r="B57" s="25" t="s">
         <v>482</v>
       </c>
-      <c r="B57" s="25" t="s">
+      <c r="C57" s="17" t="s">
         <v>483</v>
       </c>
-      <c r="C57" s="17" t="s">
-        <v>484</v>
-      </c>
       <c r="D57" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
+        <v>484</v>
+      </c>
+      <c r="B58" s="25" t="s">
         <v>485</v>
       </c>
-      <c r="B58" s="25" t="s">
+      <c r="C58" s="17" t="s">
         <v>486</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="D58" s="15" t="s">
         <v>487</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="B59" s="25" t="s">
         <v>489</v>
       </c>
-      <c r="B59" s="25" t="s">
+      <c r="C59" s="17" t="s">
         <v>490</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>491</v>
       </c>
       <c r="D59" s="15" t="s">
         <v>339</v>
@@ -9024,86 +9024,86 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
+        <v>491</v>
+      </c>
+      <c r="B60" s="29" t="s">
         <v>492</v>
       </c>
-      <c r="B60" s="29" t="s">
+      <c r="C60" s="19" t="s">
         <v>493</v>
       </c>
-      <c r="C60" s="19" t="s">
-        <v>494</v>
-      </c>
       <c r="D60" s="15" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="B61" s="25" t="s">
         <v>495</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="C61" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="D61" s="15" t="s">
         <v>497</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="B62" s="25" t="s">
         <v>499</v>
       </c>
-      <c r="B62" s="25" t="s">
+      <c r="C62" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="C62" s="17" t="s">
-        <v>501</v>
-      </c>
       <c r="D62" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
+        <v>501</v>
+      </c>
+      <c r="B63" s="25" t="s">
         <v>502</v>
       </c>
-      <c r="B63" s="25" t="s">
+      <c r="C63" s="17" t="s">
         <v>503</v>
       </c>
-      <c r="C63" s="17" t="s">
-        <v>504</v>
-      </c>
       <c r="D63" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="B64" s="25" t="s">
         <v>505</v>
       </c>
-      <c r="B64" s="25" t="s">
+      <c r="C64" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="C64" s="17" t="s">
-        <v>507</v>
-      </c>
       <c r="D64" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="B65" s="25" t="s">
         <v>508</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="C65" s="17" t="s">
         <v>509</v>
       </c>
-      <c r="C65" s="17" t="s">
-        <v>510</v>
-      </c>
       <c r="D65" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -9121,30 +9121,30 @@
     </row>
     <row r="66" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
+        <v>510</v>
+      </c>
+      <c r="B66" s="25" t="s">
         <v>511</v>
       </c>
-      <c r="B66" s="25" t="s">
+      <c r="C66" s="17" t="s">
         <v>512</v>
       </c>
-      <c r="C66" s="17" t="s">
-        <v>513</v>
-      </c>
       <c r="D66" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
+        <v>513</v>
+      </c>
+      <c r="B67" s="25" t="s">
         <v>514</v>
       </c>
-      <c r="B67" s="25" t="s">
+      <c r="C67" s="17" t="s">
         <v>515</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="D67" s="15" t="s">
         <v>516</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>517</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -9162,16 +9162,16 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
+        <v>517</v>
+      </c>
+      <c r="B68" s="25" t="s">
         <v>518</v>
       </c>
-      <c r="B68" s="25" t="s">
+      <c r="C68" s="17" t="s">
         <v>519</v>
       </c>
-      <c r="C68" s="17" t="s">
-        <v>520</v>
-      </c>
       <c r="D68" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -9189,16 +9189,16 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
+        <v>520</v>
+      </c>
+      <c r="B69" s="25" t="s">
         <v>521</v>
       </c>
-      <c r="B69" s="25" t="s">
+      <c r="C69" s="17" t="s">
         <v>522</v>
       </c>
-      <c r="C69" s="17" t="s">
+      <c r="D69" s="15" t="s">
         <v>523</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>524</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -9216,13 +9216,13 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
+        <v>524</v>
+      </c>
+      <c r="B70" s="25" t="s">
         <v>525</v>
       </c>
-      <c r="B70" s="25" t="s">
+      <c r="C70" s="19" t="s">
         <v>526</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>527</v>
       </c>
       <c r="D70" s="15" t="s">
         <v>308</v>
@@ -9243,16 +9243,16 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B71" s="25" t="s">
+        <v>527</v>
+      </c>
+      <c r="C71" s="17" t="s">
         <v>528</v>
       </c>
-      <c r="C71" s="17" t="s">
+      <c r="D71" s="15" t="s">
         <v>529</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>530</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -9270,16 +9270,16 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
+        <v>530</v>
+      </c>
+      <c r="B72" s="25" t="s">
         <v>531</v>
       </c>
-      <c r="B72" s="25" t="s">
+      <c r="C72" s="21" t="s">
         <v>532</v>
       </c>
-      <c r="C72" s="21" t="s">
-        <v>533</v>
-      </c>
       <c r="D72" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -9297,13 +9297,13 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
+        <v>533</v>
+      </c>
+      <c r="B73" s="25" t="s">
         <v>534</v>
       </c>
-      <c r="B73" s="25" t="s">
+      <c r="C73" s="17" t="s">
         <v>535</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>536</v>
       </c>
       <c r="D73" s="15" t="s">
         <v>339</v>
@@ -9324,16 +9324,16 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
+        <v>536</v>
+      </c>
+      <c r="B74" s="25" t="s">
         <v>537</v>
       </c>
-      <c r="B74" s="25" t="s">
+      <c r="C74" s="17" t="s">
         <v>538</v>
       </c>
-      <c r="C74" s="17" t="s">
-        <v>539</v>
-      </c>
       <c r="D74" s="15" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -9351,16 +9351,16 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
+        <v>539</v>
+      </c>
+      <c r="B75" s="25" t="s">
         <v>540</v>
       </c>
-      <c r="B75" s="25" t="s">
+      <c r="C75" s="17" t="s">
         <v>541</v>
       </c>
-      <c r="C75" s="17" t="s">
-        <v>542</v>
-      </c>
       <c r="D75" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -9378,16 +9378,16 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="B76" s="25" t="s">
         <v>543</v>
       </c>
-      <c r="B76" s="25" t="s">
+      <c r="C76" s="17" t="s">
         <v>544</v>
       </c>
-      <c r="C76" s="17" t="s">
-        <v>545</v>
-      </c>
       <c r="D76" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -9405,13 +9405,13 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
+        <v>545</v>
+      </c>
+      <c r="B77" s="25" t="s">
         <v>546</v>
       </c>
-      <c r="B77" s="25" t="s">
+      <c r="C77" s="17" t="s">
         <v>547</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>548</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>304</v>
@@ -9432,16 +9432,16 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
+        <v>548</v>
+      </c>
+      <c r="B78" s="25" t="s">
         <v>549</v>
       </c>
-      <c r="B78" s="25" t="s">
+      <c r="C78" s="30" t="s">
         <v>550</v>
       </c>
-      <c r="C78" s="30" t="s">
-        <v>551</v>
-      </c>
       <c r="D78" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
@@ -9459,16 +9459,16 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="25" t="s">
+        <v>551</v>
+      </c>
+      <c r="B79" s="25" t="s">
         <v>552</v>
       </c>
-      <c r="B79" s="25" t="s">
+      <c r="C79" s="19" t="s">
         <v>553</v>
       </c>
-      <c r="C79" s="19" t="s">
+      <c r="D79" s="15" t="s">
         <v>554</v>
-      </c>
-      <c r="D79" s="15" t="s">
-        <v>555</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
@@ -9486,16 +9486,16 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="B80" s="25" t="s">
         <v>556</v>
       </c>
-      <c r="B80" s="25" t="s">
+      <c r="C80" s="17" t="s">
         <v>557</v>
       </c>
-      <c r="C80" s="17" t="s">
+      <c r="D80" s="15" t="s">
         <v>558</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>559</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
@@ -9513,16 +9513,16 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="B81" s="25" t="s">
         <v>560</v>
       </c>
-      <c r="B81" s="25" t="s">
+      <c r="C81" s="17" t="s">
         <v>561</v>
       </c>
-      <c r="C81" s="17" t="s">
-        <v>562</v>
-      </c>
       <c r="D81" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
@@ -9540,10 +9540,10 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="25" t="s">
+        <v>562</v>
+      </c>
+      <c r="B82" s="25" t="s">
         <v>563</v>
-      </c>
-      <c r="B82" s="25" t="s">
-        <v>564</v>
       </c>
       <c r="C82" s="25"/>
       <c r="D82" s="15"/>
@@ -9563,16 +9563,16 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="B83" s="25" t="s">
         <v>565</v>
       </c>
-      <c r="B83" s="25" t="s">
+      <c r="C83" s="19" t="s">
         <v>566</v>
       </c>
-      <c r="C83" s="19" t="s">
+      <c r="D83" s="15" t="s">
         <v>567</v>
-      </c>
-      <c r="D83" s="15" t="s">
-        <v>568</v>
       </c>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
@@ -9590,16 +9590,16 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
+        <v>568</v>
+      </c>
+      <c r="B84" s="25" t="s">
         <v>569</v>
       </c>
-      <c r="B84" s="25" t="s">
+      <c r="C84" s="17" t="s">
         <v>570</v>
       </c>
-      <c r="C84" s="17" t="s">
+      <c r="D84" s="15" t="s">
         <v>571</v>
-      </c>
-      <c r="D84" s="15" t="s">
-        <v>572</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
@@ -9617,16 +9617,16 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
+        <v>572</v>
+      </c>
+      <c r="B85" s="25" t="s">
         <v>573</v>
       </c>
-      <c r="B85" s="25" t="s">
+      <c r="C85" s="17" t="s">
         <v>574</v>
       </c>
-      <c r="C85" s="17" t="s">
+      <c r="D85" s="15" t="s">
         <v>575</v>
-      </c>
-      <c r="D85" s="15" t="s">
-        <v>576</v>
       </c>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
@@ -9644,16 +9644,16 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
+        <v>576</v>
+      </c>
+      <c r="B86" s="25" t="s">
         <v>577</v>
       </c>
-      <c r="B86" s="25" t="s">
+      <c r="C86" s="17" t="s">
         <v>578</v>
       </c>
-      <c r="C86" s="17" t="s">
+      <c r="D86" s="15" t="s">
         <v>579</v>
-      </c>
-      <c r="D86" s="15" t="s">
-        <v>580</v>
       </c>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
@@ -9671,16 +9671,16 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
+        <v>580</v>
+      </c>
+      <c r="B87" s="25" t="s">
         <v>581</v>
       </c>
-      <c r="B87" s="25" t="s">
+      <c r="C87" s="19" t="s">
         <v>582</v>
       </c>
-      <c r="C87" s="19" t="s">
-        <v>583</v>
-      </c>
       <c r="D87" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
@@ -9698,16 +9698,16 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
+        <v>583</v>
+      </c>
+      <c r="B88" s="25" t="s">
         <v>584</v>
       </c>
-      <c r="B88" s="25" t="s">
+      <c r="C88" s="17" t="s">
         <v>585</v>
       </c>
-      <c r="C88" s="17" t="s">
+      <c r="D88" s="15" t="s">
         <v>586</v>
-      </c>
-      <c r="D88" s="15" t="s">
-        <v>587</v>
       </c>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
@@ -9725,16 +9725,16 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
+        <v>587</v>
+      </c>
+      <c r="B89" s="25" t="s">
         <v>588</v>
       </c>
-      <c r="B89" s="25" t="s">
+      <c r="C89" s="17" t="s">
         <v>589</v>
       </c>
-      <c r="C89" s="17" t="s">
+      <c r="D89" s="15" t="s">
         <v>590</v>
-      </c>
-      <c r="D89" s="15" t="s">
-        <v>591</v>
       </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
@@ -9752,16 +9752,16 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
+        <v>591</v>
+      </c>
+      <c r="B90" s="25" t="s">
         <v>592</v>
       </c>
-      <c r="B90" s="25" t="s">
+      <c r="C90" s="17" t="s">
         <v>593</v>
       </c>
-      <c r="C90" s="17" t="s">
-        <v>594</v>
-      </c>
       <c r="D90" s="15" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
@@ -9779,16 +9779,16 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="B91" s="25" t="s">
         <v>595</v>
       </c>
-      <c r="B91" s="25" t="s">
+      <c r="C91" s="17" t="s">
         <v>596</v>
       </c>
-      <c r="C91" s="17" t="s">
+      <c r="D91" s="15" t="s">
         <v>597</v>
-      </c>
-      <c r="D91" s="15" t="s">
-        <v>598</v>
       </c>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
@@ -9806,13 +9806,13 @@
     </row>
     <row r="92" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
+        <v>598</v>
+      </c>
+      <c r="B92" s="25" t="s">
         <v>599</v>
       </c>
-      <c r="B92" s="25" t="s">
+      <c r="C92" s="30" t="s">
         <v>600</v>
-      </c>
-      <c r="C92" s="30" t="s">
-        <v>601</v>
       </c>
       <c r="D92" s="15" t="s">
         <v>300</v>
@@ -9833,16 +9833,16 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
+        <v>601</v>
+      </c>
+      <c r="B93" s="25" t="s">
         <v>602</v>
       </c>
-      <c r="B93" s="25" t="s">
+      <c r="C93" s="21" t="s">
         <v>603</v>
       </c>
-      <c r="C93" s="21" t="s">
-        <v>604</v>
-      </c>
       <c r="D93" s="15" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
@@ -9860,16 +9860,16 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
+        <v>604</v>
+      </c>
+      <c r="B94" s="25" t="s">
         <v>605</v>
       </c>
-      <c r="B94" s="25" t="s">
+      <c r="C94" s="17" t="s">
         <v>606</v>
       </c>
-      <c r="C94" s="17" t="s">
+      <c r="D94" s="15" t="s">
         <v>607</v>
-      </c>
-      <c r="D94" s="15" t="s">
-        <v>608</v>
       </c>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
@@ -9887,16 +9887,16 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="B95" s="25" t="s">
         <v>609</v>
       </c>
-      <c r="B95" s="25" t="s">
+      <c r="C95" s="17" t="s">
         <v>610</v>
       </c>
-      <c r="C95" s="17" t="s">
+      <c r="D95" s="15" t="s">
         <v>611</v>
-      </c>
-      <c r="D95" s="15" t="s">
-        <v>612</v>
       </c>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
@@ -9914,13 +9914,13 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
+        <v>612</v>
+      </c>
+      <c r="B96" s="25" t="s">
         <v>613</v>
       </c>
-      <c r="B96" s="25" t="s">
+      <c r="C96" s="17" t="s">
         <v>614</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>615</v>
       </c>
       <c r="D96" s="15" t="s">
         <v>327</v>
@@ -9941,13 +9941,13 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
+        <v>615</v>
+      </c>
+      <c r="B97" s="25" t="s">
         <v>616</v>
       </c>
-      <c r="B97" s="25" t="s">
+      <c r="C97" s="17" t="s">
         <v>617</v>
-      </c>
-      <c r="C97" s="17" t="s">
-        <v>618</v>
       </c>
       <c r="D97" s="15" t="s">
         <v>300</v>
@@ -9968,16 +9968,16 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
+        <v>618</v>
+      </c>
+      <c r="B98" s="25" t="s">
         <v>619</v>
       </c>
-      <c r="B98" s="25" t="s">
+      <c r="C98" s="17" t="s">
         <v>620</v>
       </c>
-      <c r="C98" s="17" t="s">
-        <v>621</v>
-      </c>
       <c r="D98" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -9995,16 +9995,16 @@
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B99" s="25" t="s">
         <v>622</v>
       </c>
-      <c r="B99" s="25" t="s">
+      <c r="C99" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="C99" s="17" t="s">
+      <c r="D99" s="15" t="s">
         <v>624</v>
-      </c>
-      <c r="D99" s="15" t="s">
-        <v>625</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -10022,16 +10022,16 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
+        <v>625</v>
+      </c>
+      <c r="B100" s="25" t="s">
         <v>626</v>
       </c>
-      <c r="B100" s="25" t="s">
+      <c r="C100" s="17" t="s">
         <v>627</v>
       </c>
-      <c r="C100" s="17" t="s">
-        <v>628</v>
-      </c>
       <c r="D100" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
@@ -10049,16 +10049,16 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
+        <v>628</v>
+      </c>
+      <c r="B101" s="25" t="s">
         <v>629</v>
       </c>
-      <c r="B101" s="25" t="s">
+      <c r="C101" s="18" t="s">
         <v>630</v>
       </c>
-      <c r="C101" s="18" t="s">
+      <c r="D101" s="15" t="s">
         <v>631</v>
-      </c>
-      <c r="D101" s="15" t="s">
-        <v>632</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
@@ -10076,13 +10076,13 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
+        <v>632</v>
+      </c>
+      <c r="B102" s="25" t="s">
         <v>633</v>
       </c>
-      <c r="B102" s="25" t="s">
+      <c r="C102" s="17" t="s">
         <v>634</v>
-      </c>
-      <c r="C102" s="17" t="s">
-        <v>635</v>
       </c>
       <c r="D102" s="15" t="s">
         <v>308</v>
@@ -10103,16 +10103,16 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
+        <v>635</v>
+      </c>
+      <c r="B103" s="25" t="s">
         <v>636</v>
       </c>
-      <c r="B103" s="25" t="s">
+      <c r="C103" s="19" t="s">
         <v>637</v>
       </c>
-      <c r="C103" s="19" t="s">
-        <v>638</v>
-      </c>
       <c r="D103" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
@@ -10130,16 +10130,16 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
+        <v>638</v>
+      </c>
+      <c r="B104" s="25" t="s">
         <v>639</v>
       </c>
-      <c r="B104" s="25" t="s">
+      <c r="C104" s="17" t="s">
         <v>640</v>
       </c>
-      <c r="C104" s="17" t="s">
+      <c r="D104" s="15" t="s">
         <v>641</v>
-      </c>
-      <c r="D104" s="15" t="s">
-        <v>642</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
@@ -10157,16 +10157,16 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
+        <v>642</v>
+      </c>
+      <c r="B105" s="25" t="s">
         <v>643</v>
       </c>
-      <c r="B105" s="25" t="s">
+      <c r="C105" s="20" t="s">
         <v>644</v>
       </c>
-      <c r="C105" s="20" t="s">
-        <v>645</v>
-      </c>
       <c r="D105" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
@@ -10184,13 +10184,13 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
+        <v>645</v>
+      </c>
+      <c r="B106" s="25" t="s">
         <v>646</v>
       </c>
-      <c r="B106" s="25" t="s">
+      <c r="C106" s="20" t="s">
         <v>647</v>
-      </c>
-      <c r="C106" s="20" t="s">
-        <v>648</v>
       </c>
       <c r="D106" s="15" t="s">
         <v>339</v>
@@ -10211,16 +10211,16 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="25" t="s">
+        <v>648</v>
+      </c>
+      <c r="B107" s="25" t="s">
         <v>649</v>
       </c>
-      <c r="B107" s="25" t="s">
+      <c r="C107" s="32" t="s">
         <v>650</v>
       </c>
-      <c r="C107" s="32" t="s">
+      <c r="D107" s="15" t="s">
         <v>651</v>
-      </c>
-      <c r="D107" s="15" t="s">
-        <v>652</v>
       </c>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
@@ -10238,16 +10238,16 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" s="25" t="s">
+        <v>652</v>
+      </c>
+      <c r="B108" s="25" t="s">
         <v>653</v>
       </c>
-      <c r="B108" s="25" t="s">
+      <c r="C108" s="27" t="s">
         <v>654</v>
       </c>
-      <c r="C108" s="27" t="s">
+      <c r="D108" s="14" t="s">
         <v>655</v>
-      </c>
-      <c r="D108" s="14" t="s">
-        <v>656</v>
       </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
@@ -10265,13 +10265,13 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="25" t="s">
+        <v>656</v>
+      </c>
+      <c r="B109" s="25" t="s">
         <v>657</v>
       </c>
-      <c r="B109" s="25" t="s">
+      <c r="C109" s="32" t="s">
         <v>658</v>
-      </c>
-      <c r="C109" s="32" t="s">
-        <v>659</v>
       </c>
       <c r="D109" s="14" t="s">
         <v>308</v>
@@ -10292,16 +10292,16 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
+        <v>659</v>
+      </c>
+      <c r="B110" s="25" t="s">
         <v>660</v>
       </c>
-      <c r="B110" s="25" t="s">
+      <c r="C110" s="20" t="s">
         <v>661</v>
       </c>
-      <c r="C110" s="20" t="s">
-        <v>662</v>
-      </c>
       <c r="D110" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
@@ -10319,16 +10319,16 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="25" t="s">
+        <v>662</v>
+      </c>
+      <c r="B111" s="25" t="s">
         <v>663</v>
       </c>
-      <c r="B111" s="25" t="s">
+      <c r="C111" s="20" t="s">
         <v>664</v>
       </c>
-      <c r="C111" s="20" t="s">
-        <v>665</v>
-      </c>
       <c r="D111" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
@@ -10346,16 +10346,16 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
+        <v>665</v>
+      </c>
+      <c r="B112" s="25" t="s">
         <v>666</v>
       </c>
-      <c r="B112" s="25" t="s">
+      <c r="C112" s="33" t="s">
         <v>667</v>
       </c>
-      <c r="C112" s="33" t="s">
-        <v>668</v>
-      </c>
       <c r="D112" s="34" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
@@ -10373,16 +10373,16 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="25" t="s">
+        <v>668</v>
+      </c>
+      <c r="B113" s="25" t="s">
         <v>669</v>
       </c>
-      <c r="B113" s="25" t="s">
+      <c r="C113" s="35" t="s">
         <v>670</v>
       </c>
-      <c r="C113" s="35" t="s">
-        <v>671</v>
-      </c>
       <c r="D113" s="15" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
@@ -10400,13 +10400,13 @@
     </row>
     <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
+        <v>671</v>
+      </c>
+      <c r="B114" s="25" t="s">
         <v>672</v>
       </c>
-      <c r="B114" s="25" t="s">
+      <c r="C114" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="C114" s="20" t="s">
-        <v>674</v>
       </c>
       <c r="D114" s="15" t="s">
         <v>339</v>
@@ -10427,13 +10427,13 @@
     </row>
     <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="25" t="s">
+        <v>674</v>
+      </c>
+      <c r="B115" s="25" t="s">
         <v>675</v>
       </c>
-      <c r="B115" s="25" t="s">
+      <c r="C115" s="33" t="s">
         <v>676</v>
-      </c>
-      <c r="C115" s="33" t="s">
-        <v>677</v>
       </c>
       <c r="D115" s="15" t="s">
         <v>339</v>
@@ -10454,13 +10454,13 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="15" t="s">
+        <v>677</v>
+      </c>
+      <c r="B116" s="25" t="s">
         <v>678</v>
       </c>
-      <c r="B116" s="25" t="s">
+      <c r="C116" s="17" t="s">
         <v>679</v>
-      </c>
-      <c r="C116" s="17" t="s">
-        <v>680</v>
       </c>
       <c r="D116" s="15" t="s">
         <v>308</v>
@@ -10481,16 +10481,16 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="25" t="s">
+        <v>680</v>
+      </c>
+      <c r="B117" s="25" t="s">
         <v>681</v>
       </c>
-      <c r="B117" s="25" t="s">
+      <c r="C117" s="19" t="s">
         <v>682</v>
       </c>
-      <c r="C117" s="19" t="s">
-        <v>683</v>
-      </c>
       <c r="D117" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
@@ -10508,16 +10508,16 @@
     </row>
     <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
+        <v>683</v>
+      </c>
+      <c r="B118" s="25" t="s">
         <v>684</v>
       </c>
-      <c r="B118" s="25" t="s">
+      <c r="C118" s="17" t="s">
         <v>685</v>
       </c>
-      <c r="C118" s="17" t="s">
-        <v>686</v>
-      </c>
       <c r="D118" s="15" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
@@ -10535,16 +10535,16 @@
     </row>
     <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
+        <v>686</v>
+      </c>
+      <c r="B119" s="25" t="s">
         <v>687</v>
       </c>
-      <c r="B119" s="25" t="s">
+      <c r="C119" s="19" t="s">
         <v>688</v>
       </c>
-      <c r="C119" s="19" t="s">
-        <v>689</v>
-      </c>
       <c r="D119" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
@@ -10562,16 +10562,16 @@
     </row>
     <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="25" t="s">
+        <v>689</v>
+      </c>
+      <c r="B120" s="25" t="s">
         <v>690</v>
       </c>
-      <c r="B120" s="25" t="s">
+      <c r="C120" s="19" t="s">
         <v>691</v>
       </c>
-      <c r="C120" s="19" t="s">
-        <v>692</v>
-      </c>
       <c r="D120" s="34" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
@@ -10589,13 +10589,13 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" s="15" t="s">
+        <v>692</v>
+      </c>
+      <c r="B121" s="25" t="s">
         <v>693</v>
       </c>
-      <c r="B121" s="25" t="s">
+      <c r="C121" s="17" t="s">
         <v>694</v>
-      </c>
-      <c r="C121" s="17" t="s">
-        <v>695</v>
       </c>
       <c r="D121" s="15" t="s">
         <v>308</v>
@@ -10616,13 +10616,13 @@
     </row>
     <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
+        <v>695</v>
+      </c>
+      <c r="B122" s="25" t="s">
         <v>696</v>
       </c>
-      <c r="B122" s="25" t="s">
+      <c r="C122" s="19" t="s">
         <v>697</v>
-      </c>
-      <c r="C122" s="19" t="s">
-        <v>698</v>
       </c>
       <c r="D122" s="15" t="s">
         <v>339</v>
@@ -10643,16 +10643,16 @@
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" s="15" t="s">
+        <v>698</v>
+      </c>
+      <c r="B123" s="25" t="s">
         <v>699</v>
       </c>
-      <c r="B123" s="25" t="s">
+      <c r="C123" s="17" t="s">
         <v>700</v>
       </c>
-      <c r="C123" s="17" t="s">
-        <v>701</v>
-      </c>
       <c r="D123" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
@@ -10670,16 +10670,16 @@
     </row>
     <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" s="15" t="s">
+        <v>701</v>
+      </c>
+      <c r="B124" s="25" t="s">
         <v>702</v>
       </c>
-      <c r="B124" s="25" t="s">
+      <c r="C124" s="17" t="s">
         <v>703</v>
       </c>
-      <c r="C124" s="17" t="s">
-        <v>704</v>
-      </c>
       <c r="D124" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
@@ -10697,16 +10697,16 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
+        <v>704</v>
+      </c>
+      <c r="B125" s="25" t="s">
         <v>705</v>
       </c>
-      <c r="B125" s="25" t="s">
+      <c r="C125" s="17" t="s">
         <v>706</v>
       </c>
-      <c r="C125" s="17" t="s">
+      <c r="D125" s="15" t="s">
         <v>707</v>
-      </c>
-      <c r="D125" s="15" t="s">
-        <v>708</v>
       </c>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
@@ -10724,16 +10724,16 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
+        <v>708</v>
+      </c>
+      <c r="B126" s="25" t="s">
         <v>709</v>
       </c>
-      <c r="B126" s="25" t="s">
+      <c r="C126" s="17" t="s">
         <v>710</v>
       </c>
-      <c r="C126" s="17" t="s">
-        <v>711</v>
-      </c>
       <c r="D126" s="15" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
@@ -10751,16 +10751,16 @@
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" s="25" t="s">
+        <v>711</v>
+      </c>
+      <c r="B127" s="25" t="s">
         <v>712</v>
       </c>
-      <c r="B127" s="25" t="s">
+      <c r="C127" s="19" t="s">
         <v>713</v>
       </c>
-      <c r="C127" s="19" t="s">
-        <v>714</v>
-      </c>
       <c r="D127" s="26" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
@@ -10778,16 +10778,16 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
+        <v>714</v>
+      </c>
+      <c r="B128" s="25" t="s">
         <v>715</v>
       </c>
-      <c r="B128" s="25" t="s">
+      <c r="C128" s="17" t="s">
         <v>716</v>
       </c>
-      <c r="C128" s="17" t="s">
-        <v>717</v>
-      </c>
       <c r="D128" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
@@ -10805,16 +10805,16 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" s="25" t="s">
+        <v>717</v>
+      </c>
+      <c r="B129" s="25" t="s">
         <v>718</v>
       </c>
-      <c r="B129" s="25" t="s">
+      <c r="C129" s="27" t="s">
         <v>719</v>
       </c>
-      <c r="C129" s="27" t="s">
-        <v>720</v>
-      </c>
       <c r="D129" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
@@ -10832,13 +10832,13 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" s="15" t="s">
+        <v>720</v>
+      </c>
+      <c r="B130" s="25" t="s">
         <v>721</v>
       </c>
-      <c r="B130" s="25" t="s">
+      <c r="C130" s="17" t="s">
         <v>722</v>
-      </c>
-      <c r="C130" s="17" t="s">
-        <v>723</v>
       </c>
       <c r="D130" s="15" t="s">
         <v>304</v>
@@ -10859,13 +10859,13 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
+        <v>723</v>
+      </c>
+      <c r="B131" s="25" t="s">
         <v>724</v>
       </c>
-      <c r="B131" s="25" t="s">
+      <c r="C131" s="17" t="s">
         <v>725</v>
-      </c>
-      <c r="C131" s="17" t="s">
-        <v>726</v>
       </c>
       <c r="D131" s="15" t="s">
         <v>308</v>
@@ -10886,13 +10886,13 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" s="15" t="s">
+        <v>726</v>
+      </c>
+      <c r="B132" s="25" t="s">
         <v>727</v>
       </c>
-      <c r="B132" s="25" t="s">
+      <c r="C132" s="17" t="s">
         <v>728</v>
-      </c>
-      <c r="C132" s="17" t="s">
-        <v>729</v>
       </c>
       <c r="D132" s="15" t="s">
         <v>304</v>
@@ -10913,16 +10913,16 @@
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" s="25" t="s">
+        <v>729</v>
+      </c>
+      <c r="B133" s="25" t="s">
         <v>730</v>
       </c>
-      <c r="B133" s="25" t="s">
+      <c r="C133" s="27" t="s">
         <v>731</v>
       </c>
-      <c r="C133" s="27" t="s">
+      <c r="D133" s="14" t="s">
         <v>732</v>
-      </c>
-      <c r="D133" s="14" t="s">
-        <v>733</v>
       </c>
       <c r="E133" s="3"/>
       <c r="F133" s="3"/>
@@ -10940,16 +10940,16 @@
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" s="25" t="s">
+        <v>733</v>
+      </c>
+      <c r="B134" s="25" t="s">
         <v>734</v>
       </c>
-      <c r="B134" s="25" t="s">
+      <c r="C134" s="27" t="s">
         <v>735</v>
       </c>
-      <c r="C134" s="27" t="s">
+      <c r="D134" s="28" t="s">
         <v>736</v>
-      </c>
-      <c r="D134" s="28" t="s">
-        <v>737</v>
       </c>
       <c r="E134" s="3"/>
       <c r="F134" s="3"/>
@@ -10967,13 +10967,13 @@
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" s="15" t="s">
+        <v>737</v>
+      </c>
+      <c r="B135" s="25" t="s">
         <v>738</v>
       </c>
-      <c r="B135" s="25" t="s">
+      <c r="C135" s="17" t="s">
         <v>739</v>
-      </c>
-      <c r="C135" s="17" t="s">
-        <v>740</v>
       </c>
       <c r="D135" s="15" t="s">
         <v>308</v>
@@ -10994,16 +10994,16 @@
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" s="25" t="s">
+        <v>740</v>
+      </c>
+      <c r="B136" s="25" t="s">
         <v>741</v>
       </c>
-      <c r="B136" s="25" t="s">
+      <c r="C136" s="27" t="s">
         <v>742</v>
       </c>
-      <c r="C136" s="27" t="s">
-        <v>743</v>
-      </c>
       <c r="D136" s="15" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E136" s="3"/>
       <c r="F136" s="3"/>
@@ -11021,13 +11021,13 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" s="15" t="s">
+        <v>743</v>
+      </c>
+      <c r="B137" s="25" t="s">
         <v>744</v>
       </c>
-      <c r="B137" s="25" t="s">
+      <c r="C137" s="19" t="s">
         <v>745</v>
-      </c>
-      <c r="C137" s="19" t="s">
-        <v>746</v>
       </c>
       <c r="D137" s="15" t="s">
         <v>339</v>
@@ -11048,16 +11048,16 @@
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" s="25" t="s">
+        <v>746</v>
+      </c>
+      <c r="B138" s="36" t="s">
         <v>747</v>
       </c>
-      <c r="B138" s="36" t="s">
+      <c r="C138" s="27" t="s">
         <v>748</v>
       </c>
-      <c r="C138" s="27" t="s">
-        <v>749</v>
-      </c>
       <c r="D138" s="37" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E138" s="3"/>
       <c r="F138" s="3"/>
@@ -11075,16 +11075,16 @@
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" s="25" t="s">
+        <v>749</v>
+      </c>
+      <c r="B139" s="25" t="s">
         <v>750</v>
       </c>
-      <c r="B139" s="25" t="s">
+      <c r="C139" s="19" t="s">
         <v>751</v>
       </c>
-      <c r="C139" s="19" t="s">
-        <v>752</v>
-      </c>
       <c r="D139" s="34" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E139" s="3"/>
       <c r="F139" s="3"/>
@@ -11102,13 +11102,13 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
+        <v>752</v>
+      </c>
+      <c r="B140" s="25" t="s">
         <v>753</v>
       </c>
-      <c r="B140" s="25" t="s">
+      <c r="C140" s="17" t="s">
         <v>754</v>
-      </c>
-      <c r="C140" s="17" t="s">
-        <v>755</v>
       </c>
       <c r="D140" s="15" t="s">
         <v>327</v>
@@ -11129,16 +11129,16 @@
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
+        <v>755</v>
+      </c>
+      <c r="B141" s="25" t="s">
         <v>756</v>
       </c>
-      <c r="B141" s="25" t="s">
+      <c r="C141" s="17" t="s">
         <v>757</v>
       </c>
-      <c r="C141" s="17" t="s">
+      <c r="D141" s="15" t="s">
         <v>758</v>
-      </c>
-      <c r="D141" s="15" t="s">
-        <v>759</v>
       </c>
       <c r="E141" s="3"/>
       <c r="F141" s="3"/>
@@ -11156,16 +11156,16 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" s="15" t="s">
+        <v>759</v>
+      </c>
+      <c r="B142" s="25" t="s">
         <v>760</v>
       </c>
-      <c r="B142" s="25" t="s">
+      <c r="C142" s="17" t="s">
         <v>761</v>
       </c>
-      <c r="C142" s="17" t="s">
-        <v>762</v>
-      </c>
       <c r="D142" s="15" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E142" s="3"/>
       <c r="F142" s="3"/>
@@ -11183,13 +11183,13 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" s="15" t="s">
+        <v>762</v>
+      </c>
+      <c r="B143" s="25" t="s">
         <v>763</v>
       </c>
-      <c r="B143" s="25" t="s">
+      <c r="C143" s="17" t="s">
         <v>764</v>
-      </c>
-      <c r="C143" s="17" t="s">
-        <v>765</v>
       </c>
       <c r="D143" s="15" t="s">
         <v>308</v>
@@ -11210,13 +11210,13 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" s="15" t="s">
+        <v>765</v>
+      </c>
+      <c r="B144" s="25" t="s">
         <v>766</v>
       </c>
-      <c r="B144" s="25" t="s">
+      <c r="C144" s="17" t="s">
         <v>767</v>
-      </c>
-      <c r="C144" s="17" t="s">
-        <v>768</v>
       </c>
       <c r="D144" s="15" t="s">
         <v>339</v>
@@ -11237,16 +11237,16 @@
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" s="25" t="s">
+        <v>768</v>
+      </c>
+      <c r="B145" s="25" t="s">
         <v>769</v>
       </c>
-      <c r="B145" s="25" t="s">
+      <c r="C145" s="27" t="s">
         <v>770</v>
       </c>
-      <c r="C145" s="27" t="s">
+      <c r="D145" s="15" t="s">
         <v>771</v>
-      </c>
-      <c r="D145" s="15" t="s">
-        <v>772</v>
       </c>
       <c r="E145" s="3"/>
       <c r="F145" s="3"/>
@@ -11264,16 +11264,16 @@
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" s="15" t="s">
+        <v>772</v>
+      </c>
+      <c r="B146" s="25" t="s">
         <v>773</v>
       </c>
-      <c r="B146" s="25" t="s">
+      <c r="C146" s="17" t="s">
         <v>774</v>
       </c>
-      <c r="C146" s="17" t="s">
-        <v>775</v>
-      </c>
       <c r="D146" s="15" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
@@ -11291,16 +11291,16 @@
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" s="15" t="s">
+        <v>775</v>
+      </c>
+      <c r="B147" s="25" t="s">
         <v>776</v>
       </c>
-      <c r="B147" s="25" t="s">
+      <c r="C147" s="17" t="s">
         <v>777</v>
       </c>
-      <c r="C147" s="17" t="s">
-        <v>778</v>
-      </c>
       <c r="D147" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E147" s="3"/>
       <c r="F147" s="3"/>
@@ -11318,16 +11318,16 @@
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" s="15" t="s">
+        <v>778</v>
+      </c>
+      <c r="B148" s="25" t="s">
         <v>779</v>
       </c>
-      <c r="B148" s="25" t="s">
+      <c r="C148" s="17" t="s">
         <v>780</v>
       </c>
-      <c r="C148" s="17" t="s">
+      <c r="D148" s="15" t="s">
         <v>781</v>
-      </c>
-      <c r="D148" s="15" t="s">
-        <v>782</v>
       </c>
       <c r="E148" s="3"/>
       <c r="F148" s="3"/>
@@ -11345,16 +11345,16 @@
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" s="15" t="s">
+        <v>782</v>
+      </c>
+      <c r="B149" s="25" t="s">
         <v>783</v>
       </c>
-      <c r="B149" s="25" t="s">
-        <v>784</v>
-      </c>
       <c r="C149" s="17" t="s">
+        <v>780</v>
+      </c>
+      <c r="D149" s="15" t="s">
         <v>781</v>
-      </c>
-      <c r="D149" s="15" t="s">
-        <v>782</v>
       </c>
       <c r="E149" s="3"/>
       <c r="F149" s="3"/>
@@ -11372,16 +11372,16 @@
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" s="15" t="s">
+        <v>784</v>
+      </c>
+      <c r="B150" s="25" t="s">
         <v>785</v>
       </c>
-      <c r="B150" s="25" t="s">
-        <v>786</v>
-      </c>
       <c r="C150" s="17" t="s">
+        <v>780</v>
+      </c>
+      <c r="D150" s="15" t="s">
         <v>781</v>
-      </c>
-      <c r="D150" s="15" t="s">
-        <v>782</v>
       </c>
       <c r="E150" s="3"/>
       <c r="F150" s="3"/>
@@ -11399,16 +11399,16 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" s="15" t="s">
+        <v>786</v>
+      </c>
+      <c r="B151" s="25" t="s">
         <v>787</v>
       </c>
-      <c r="B151" s="25" t="s">
-        <v>788</v>
-      </c>
       <c r="C151" s="17" t="s">
+        <v>780</v>
+      </c>
+      <c r="D151" s="15" t="s">
         <v>781</v>
-      </c>
-      <c r="D151" s="15" t="s">
-        <v>782</v>
       </c>
       <c r="E151" s="3"/>
       <c r="F151" s="3"/>
@@ -11426,16 +11426,16 @@
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" s="36" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B152" s="25" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C152" s="17" t="s">
+        <v>780</v>
+      </c>
+      <c r="D152" s="15" t="s">
         <v>781</v>
-      </c>
-      <c r="D152" s="15" t="s">
-        <v>782</v>
       </c>
       <c r="E152" s="3"/>
       <c r="F152" s="3"/>
@@ -11453,16 +11453,16 @@
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" s="15" t="s">
+        <v>789</v>
+      </c>
+      <c r="B153" s="25" t="s">
         <v>790</v>
       </c>
-      <c r="B153" s="25" t="s">
+      <c r="C153" s="17" t="s">
         <v>791</v>
       </c>
-      <c r="C153" s="17" t="s">
+      <c r="D153" s="38" t="s">
         <v>792</v>
-      </c>
-      <c r="D153" s="38" t="s">
-        <v>793</v>
       </c>
       <c r="E153" s="3"/>
       <c r="F153" s="3"/>
@@ -11480,16 +11480,16 @@
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" s="25" t="s">
+        <v>793</v>
+      </c>
+      <c r="B154" s="25" t="s">
         <v>794</v>
       </c>
-      <c r="B154" s="25" t="s">
+      <c r="C154" s="39" t="s">
         <v>795</v>
       </c>
-      <c r="C154" s="39" t="s">
-        <v>796</v>
-      </c>
       <c r="D154" s="15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E154" s="3"/>
       <c r="F154" s="3"/>
@@ -11507,13 +11507,13 @@
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" s="25" t="s">
+        <v>796</v>
+      </c>
+      <c r="B155" s="25" t="s">
         <v>797</v>
       </c>
-      <c r="B155" s="25" t="s">
+      <c r="C155" s="27" t="s">
         <v>798</v>
-      </c>
-      <c r="C155" s="27" t="s">
-        <v>799</v>
       </c>
       <c r="D155" s="15" t="s">
         <v>308</v>
@@ -11534,16 +11534,16 @@
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" s="25" t="s">
+        <v>799</v>
+      </c>
+      <c r="B156" s="25" t="s">
         <v>800</v>
       </c>
-      <c r="B156" s="25" t="s">
+      <c r="C156" s="27" t="s">
         <v>801</v>
       </c>
-      <c r="C156" s="27" t="s">
+      <c r="D156" s="14" t="s">
         <v>802</v>
-      </c>
-      <c r="D156" s="14" t="s">
-        <v>803</v>
       </c>
       <c r="E156" s="3"/>
       <c r="F156" s="3"/>
@@ -11561,16 +11561,16 @@
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157" s="15" t="s">
+        <v>803</v>
+      </c>
+      <c r="B157" s="25" t="s">
         <v>804</v>
       </c>
-      <c r="B157" s="25" t="s">
+      <c r="C157" s="17" t="s">
         <v>805</v>
       </c>
-      <c r="C157" s="17" t="s">
-        <v>806</v>
-      </c>
       <c r="D157" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E157" s="3"/>
       <c r="F157" s="3"/>
@@ -11588,16 +11588,16 @@
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A158" s="25" t="s">
+        <v>806</v>
+      </c>
+      <c r="B158" s="25" t="s">
         <v>807</v>
       </c>
-      <c r="B158" s="25" t="s">
+      <c r="C158" s="27" t="s">
         <v>808</v>
       </c>
-      <c r="C158" s="27" t="s">
+      <c r="D158" s="14" t="s">
         <v>809</v>
-      </c>
-      <c r="D158" s="14" t="s">
-        <v>810</v>
       </c>
       <c r="E158" s="3"/>
       <c r="F158" s="3"/>
@@ -11615,13 +11615,13 @@
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" s="15" t="s">
+        <v>810</v>
+      </c>
+      <c r="B159" s="25" t="s">
         <v>811</v>
       </c>
-      <c r="B159" s="25" t="s">
+      <c r="C159" s="17" t="s">
         <v>812</v>
-      </c>
-      <c r="C159" s="17" t="s">
-        <v>813</v>
       </c>
       <c r="D159" s="15" t="s">
         <v>300</v>
@@ -11642,16 +11642,16 @@
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160" s="15" t="s">
+        <v>813</v>
+      </c>
+      <c r="B160" s="25" t="s">
         <v>814</v>
       </c>
-      <c r="B160" s="25" t="s">
+      <c r="C160" s="20" t="s">
         <v>815</v>
       </c>
-      <c r="C160" s="20" t="s">
+      <c r="D160" s="15" t="s">
         <v>816</v>
-      </c>
-      <c r="D160" s="15" t="s">
-        <v>817</v>
       </c>
       <c r="E160" s="3"/>
       <c r="F160" s="3"/>
@@ -11669,16 +11669,16 @@
     </row>
     <row r="161" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
+        <v>817</v>
+      </c>
+      <c r="B161" s="25" t="s">
         <v>818</v>
       </c>
-      <c r="B161" s="25" t="s">
+      <c r="C161" s="32" t="s">
         <v>819</v>
       </c>
-      <c r="C161" s="32" t="s">
+      <c r="D161" s="14" t="s">
         <v>820</v>
-      </c>
-      <c r="D161" s="14" t="s">
-        <v>821</v>
       </c>
       <c r="E161" s="3"/>
       <c r="F161" s="3"/>
@@ -11696,16 +11696,16 @@
     </row>
     <row r="162" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A162" s="25" t="s">
+        <v>821</v>
+      </c>
+      <c r="B162" s="25" t="s">
         <v>822</v>
       </c>
-      <c r="B162" s="25" t="s">
+      <c r="C162" s="32" t="s">
         <v>823</v>
       </c>
-      <c r="C162" s="32" t="s">
+      <c r="D162" s="40" t="s">
         <v>824</v>
-      </c>
-      <c r="D162" s="40" t="s">
-        <v>825</v>
       </c>
       <c r="E162" s="3"/>
       <c r="F162" s="3"/>
@@ -11723,16 +11723,16 @@
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A163" s="15" t="s">
+        <v>825</v>
+      </c>
+      <c r="B163" s="25" t="s">
         <v>826</v>
       </c>
-      <c r="B163" s="25" t="s">
+      <c r="C163" s="33" t="s">
         <v>827</v>
       </c>
-      <c r="C163" s="33" t="s">
+      <c r="D163" s="15" t="s">
         <v>828</v>
-      </c>
-      <c r="D163" s="15" t="s">
-        <v>829</v>
       </c>
       <c r="E163" s="3"/>
       <c r="F163" s="3"/>
@@ -11750,16 +11750,16 @@
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A164" s="15" t="s">
+        <v>829</v>
+      </c>
+      <c r="B164" s="25" t="s">
         <v>830</v>
       </c>
-      <c r="B164" s="25" t="s">
+      <c r="C164" s="20" t="s">
         <v>831</v>
       </c>
-      <c r="C164" s="20" t="s">
-        <v>832</v>
-      </c>
       <c r="D164" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E164" s="3"/>
       <c r="F164" s="3"/>
@@ -11777,16 +11777,16 @@
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A165" s="36" t="s">
+        <v>832</v>
+      </c>
+      <c r="B165" s="25" t="s">
         <v>833</v>
       </c>
-      <c r="B165" s="25" t="s">
+      <c r="C165" s="32" t="s">
         <v>834</v>
       </c>
-      <c r="C165" s="32" t="s">
+      <c r="D165" s="15" t="s">
         <v>835</v>
-      </c>
-      <c r="D165" s="15" t="s">
-        <v>836</v>
       </c>
       <c r="E165" s="3"/>
       <c r="F165" s="3"/>
@@ -11804,16 +11804,16 @@
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A166" s="25" t="s">
+        <v>836</v>
+      </c>
+      <c r="B166" s="25" t="s">
         <v>837</v>
       </c>
-      <c r="B166" s="25" t="s">
+      <c r="C166" s="33" t="s">
         <v>838</v>
       </c>
-      <c r="C166" s="33" t="s">
-        <v>839</v>
-      </c>
       <c r="D166" s="34" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E166" s="3"/>
       <c r="F166" s="3"/>
@@ -11831,13 +11831,13 @@
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A167" s="15" t="s">
+        <v>839</v>
+      </c>
+      <c r="B167" s="25" t="s">
         <v>840</v>
       </c>
-      <c r="B167" s="25" t="s">
+      <c r="C167" s="17" t="s">
         <v>841</v>
-      </c>
-      <c r="C167" s="17" t="s">
-        <v>842</v>
       </c>
       <c r="D167" s="15" t="s">
         <v>308</v>
@@ -11858,13 +11858,13 @@
     </row>
     <row r="168" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="15" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B168" s="36" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C168" s="20" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D168" s="15" t="s">
         <v>339</v>
@@ -11872,13 +11872,13 @@
     </row>
     <row r="169" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="40" t="s">
+        <v>916</v>
+      </c>
+      <c r="B169" s="41" t="s">
+        <v>915</v>
+      </c>
+      <c r="C169" s="48" t="s">
         <v>917</v>
-      </c>
-      <c r="B169" s="41" t="s">
-        <v>916</v>
-      </c>
-      <c r="C169" s="48" t="s">
-        <v>918</v>
       </c>
       <c r="D169" s="28" t="s">
         <v>339</v>
@@ -11886,10 +11886,10 @@
     </row>
     <row r="170" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="40" t="s">
+        <v>842</v>
+      </c>
+      <c r="B170" s="42" t="s">
         <v>843</v>
-      </c>
-      <c r="B170" s="42" t="s">
-        <v>844</v>
       </c>
       <c r="C170" s="30"/>
       <c r="D170" s="40" t="s">
@@ -11898,16 +11898,16 @@
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A171" s="43" t="s">
+        <v>844</v>
+      </c>
+      <c r="B171" s="44" t="s">
         <v>845</v>
       </c>
-      <c r="B171" s="44" t="s">
+      <c r="C171" s="45" t="s">
         <v>846</v>
       </c>
-      <c r="C171" s="45" t="s">
-        <v>847</v>
-      </c>
       <c r="D171" s="43" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E171" s="3"/>
       <c r="F171" s="3"/>
@@ -11925,13 +11925,13 @@
     </row>
     <row r="172" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="41" t="s">
+        <v>847</v>
+      </c>
+      <c r="B172" s="41" t="s">
         <v>848</v>
       </c>
-      <c r="B172" s="41" t="s">
+      <c r="C172" s="46" t="s">
         <v>849</v>
-      </c>
-      <c r="C172" s="46" t="s">
-        <v>850</v>
       </c>
       <c r="D172" s="28" t="s">
         <v>346</v>
@@ -11939,13 +11939,13 @@
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A173" s="25" t="s">
+        <v>850</v>
+      </c>
+      <c r="B173" s="36" t="s">
         <v>851</v>
       </c>
-      <c r="B173" s="36" t="s">
+      <c r="C173" s="32" t="s">
         <v>852</v>
-      </c>
-      <c r="C173" s="32" t="s">
-        <v>853</v>
       </c>
       <c r="D173" s="14" t="s">
         <v>346</v>
@@ -11966,16 +11966,16 @@
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A174" s="15" t="s">
+        <v>853</v>
+      </c>
+      <c r="B174" s="25" t="s">
         <v>854</v>
       </c>
-      <c r="B174" s="25" t="s">
+      <c r="C174" s="20" t="s">
         <v>855</v>
       </c>
-      <c r="C174" s="20" t="s">
-        <v>856</v>
-      </c>
       <c r="D174" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E174" s="3"/>
       <c r="F174" s="3"/>
@@ -11993,13 +11993,13 @@
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A175" s="15" t="s">
+        <v>856</v>
+      </c>
+      <c r="B175" s="25" t="s">
         <v>857</v>
       </c>
-      <c r="B175" s="25" t="s">
+      <c r="C175" s="20" t="s">
         <v>858</v>
-      </c>
-      <c r="C175" s="20" t="s">
-        <v>859</v>
       </c>
       <c r="D175" s="15" t="s">
         <v>308</v>
@@ -12020,13 +12020,13 @@
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A176" s="15" t="s">
+        <v>859</v>
+      </c>
+      <c r="B176" s="25" t="s">
         <v>860</v>
       </c>
-      <c r="B176" s="25" t="s">
+      <c r="C176" s="33" t="s">
         <v>861</v>
-      </c>
-      <c r="C176" s="33" t="s">
-        <v>862</v>
       </c>
       <c r="D176" s="15" t="s">
         <v>339</v>
@@ -12047,16 +12047,16 @@
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A177" s="25" t="s">
+        <v>862</v>
+      </c>
+      <c r="B177" s="25" t="s">
         <v>863</v>
       </c>
-      <c r="B177" s="25" t="s">
+      <c r="C177" s="32" t="s">
         <v>864</v>
       </c>
-      <c r="C177" s="32" t="s">
-        <v>865</v>
-      </c>
       <c r="D177" s="15" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E177" s="3"/>
       <c r="F177" s="3"/>
@@ -12074,16 +12074,16 @@
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A178" s="15" t="s">
+        <v>865</v>
+      </c>
+      <c r="B178" s="25" t="s">
         <v>866</v>
       </c>
-      <c r="B178" s="25" t="s">
+      <c r="C178" s="20" t="s">
         <v>867</v>
       </c>
-      <c r="C178" s="20" t="s">
+      <c r="D178" s="16" t="s">
         <v>868</v>
-      </c>
-      <c r="D178" s="16" t="s">
-        <v>869</v>
       </c>
       <c r="E178" s="3"/>
       <c r="F178" s="3"/>
@@ -12101,16 +12101,16 @@
     </row>
     <row r="179" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A179" s="25" t="s">
+        <v>869</v>
+      </c>
+      <c r="B179" s="25" t="s">
         <v>870</v>
       </c>
-      <c r="B179" s="25" t="s">
+      <c r="C179" s="18" t="s">
         <v>871</v>
       </c>
-      <c r="C179" s="18" t="s">
-        <v>872</v>
-      </c>
       <c r="D179" s="14" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E179" s="3"/>
       <c r="F179" s="3"/>
@@ -12128,13 +12128,13 @@
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A180" s="15" t="s">
+        <v>872</v>
+      </c>
+      <c r="B180" s="25" t="s">
         <v>873</v>
       </c>
-      <c r="B180" s="25" t="s">
+      <c r="C180" s="33" t="s">
         <v>874</v>
-      </c>
-      <c r="C180" s="33" t="s">
-        <v>875</v>
       </c>
       <c r="D180" s="15" t="s">
         <v>339</v>
@@ -12155,13 +12155,13 @@
     </row>
     <row r="181" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A181" s="15" t="s">
+        <v>875</v>
+      </c>
+      <c r="B181" s="25" t="s">
         <v>876</v>
       </c>
-      <c r="B181" s="25" t="s">
+      <c r="C181" s="20" t="s">
         <v>877</v>
-      </c>
-      <c r="C181" s="20" t="s">
-        <v>878</v>
       </c>
       <c r="D181" s="15" t="s">
         <v>335</v>
@@ -12182,16 +12182,16 @@
     </row>
     <row r="182" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A182" s="15" t="s">
+        <v>878</v>
+      </c>
+      <c r="B182" s="25" t="s">
         <v>879</v>
       </c>
-      <c r="B182" s="25" t="s">
+      <c r="C182" s="20" t="s">
         <v>880</v>
       </c>
-      <c r="C182" s="20" t="s">
-        <v>881</v>
-      </c>
       <c r="D182" s="15" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E182" s="3"/>
       <c r="F182" s="3"/>
@@ -12209,16 +12209,16 @@
     </row>
     <row r="183" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A183" s="15" t="s">
+        <v>881</v>
+      </c>
+      <c r="B183" s="25" t="s">
         <v>882</v>
       </c>
-      <c r="B183" s="25" t="s">
+      <c r="C183" s="20" t="s">
         <v>883</v>
       </c>
-      <c r="C183" s="20" t="s">
-        <v>884</v>
-      </c>
       <c r="D183" s="15" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E183" s="3"/>
       <c r="F183" s="3"/>
@@ -12236,13 +12236,13 @@
     </row>
     <row r="184" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A184" s="15" t="s">
+        <v>884</v>
+      </c>
+      <c r="B184" s="25" t="s">
         <v>885</v>
       </c>
-      <c r="B184" s="25" t="s">
+      <c r="C184" s="20" t="s">
         <v>886</v>
-      </c>
-      <c r="C184" s="20" t="s">
-        <v>887</v>
       </c>
       <c r="D184" s="15" t="s">
         <v>308</v>
@@ -12263,16 +12263,16 @@
     </row>
     <row r="185" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A185" s="15" t="s">
+        <v>887</v>
+      </c>
+      <c r="B185" s="25" t="s">
         <v>888</v>
       </c>
-      <c r="B185" s="25" t="s">
+      <c r="C185" s="20" t="s">
         <v>889</v>
       </c>
-      <c r="C185" s="20" t="s">
-        <v>890</v>
-      </c>
       <c r="D185" s="15" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E185" s="3"/>
       <c r="F185" s="3"/>
@@ -12290,16 +12290,16 @@
     </row>
     <row r="186" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A186" s="15" t="s">
+        <v>890</v>
+      </c>
+      <c r="B186" s="25" t="s">
         <v>891</v>
       </c>
-      <c r="B186" s="25" t="s">
+      <c r="C186" s="20" t="s">
         <v>892</v>
       </c>
-      <c r="C186" s="20" t="s">
-        <v>893</v>
-      </c>
       <c r="D186" s="15" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="E186" s="3"/>
       <c r="F186" s="3"/>
@@ -12317,16 +12317,16 @@
     </row>
     <row r="187" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A187" s="15" t="s">
+        <v>893</v>
+      </c>
+      <c r="B187" s="25" t="s">
         <v>894</v>
       </c>
-      <c r="B187" s="25" t="s">
+      <c r="C187" s="33" t="s">
         <v>895</v>
       </c>
-      <c r="C187" s="33" t="s">
+      <c r="D187" s="34" t="s">
         <v>896</v>
-      </c>
-      <c r="D187" s="34" t="s">
-        <v>897</v>
       </c>
       <c r="E187" s="3"/>
       <c r="F187" s="3"/>
@@ -12344,13 +12344,13 @@
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A188" s="25" t="s">
+        <v>897</v>
+      </c>
+      <c r="B188" s="25" t="s">
         <v>898</v>
       </c>
-      <c r="B188" s="25" t="s">
+      <c r="C188" s="47" t="s">
         <v>899</v>
-      </c>
-      <c r="C188" s="47" t="s">
-        <v>900</v>
       </c>
       <c r="D188" s="15" t="s">
         <v>335</v>
@@ -12371,13 +12371,13 @@
     </row>
     <row r="189" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A189" s="25" t="s">
+        <v>900</v>
+      </c>
+      <c r="B189" s="25" t="s">
         <v>901</v>
       </c>
-      <c r="B189" s="25" t="s">
+      <c r="C189" s="32" t="s">
         <v>902</v>
-      </c>
-      <c r="C189" s="32" t="s">
-        <v>903</v>
       </c>
       <c r="D189" s="15" t="s">
         <v>331</v>
@@ -12398,16 +12398,16 @@
     </row>
     <row r="190" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A190" s="25" t="s">
+        <v>903</v>
+      </c>
+      <c r="B190" s="25" t="s">
         <v>904</v>
       </c>
-      <c r="B190" s="25" t="s">
+      <c r="C190" s="32" t="s">
         <v>905</v>
       </c>
-      <c r="C190" s="32" t="s">
+      <c r="D190" s="15" t="s">
         <v>906</v>
-      </c>
-      <c r="D190" s="15" t="s">
-        <v>907</v>
       </c>
       <c r="E190" s="3"/>
       <c r="F190" s="3"/>
@@ -12425,13 +12425,13 @@
     </row>
     <row r="191" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A191" s="15" t="s">
+        <v>907</v>
+      </c>
+      <c r="B191" s="25" t="s">
         <v>908</v>
       </c>
-      <c r="B191" s="25" t="s">
+      <c r="C191" s="20" t="s">
         <v>909</v>
-      </c>
-      <c r="C191" s="20" t="s">
-        <v>910</v>
       </c>
       <c r="D191" s="15" t="s">
         <v>304</v>
@@ -12452,16 +12452,16 @@
     </row>
     <row r="192" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A192" s="25" t="s">
+        <v>910</v>
+      </c>
+      <c r="B192" s="36" t="s">
         <v>911</v>
       </c>
-      <c r="B192" s="36" t="s">
+      <c r="C192" s="27" t="s">
         <v>912</v>
       </c>
-      <c r="C192" s="27" t="s">
+      <c r="D192" s="16" t="s">
         <v>913</v>
-      </c>
-      <c r="D192" s="16" t="s">
-        <v>914</v>
       </c>
       <c r="E192" s="3"/>
       <c r="F192" s="3"/>
@@ -27690,44 +27690,44 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
+        <v>930</v>
+      </c>
+      <c r="B1" s="51" t="s">
         <v>931</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="C1" s="51" t="s">
+        <v>933</v>
+      </c>
+      <c r="D1" s="51" t="s">
         <v>932</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>934</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
+        <v>928</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>929</v>
       </c>
-      <c r="B2" s="53" t="s">
-        <v>930</v>
-      </c>
       <c r="C2" s="53" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C3" s="53" t="s">
+        <v>935</v>
+      </c>
+      <c r="D3" s="53" t="s">
         <v>936</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>937</v>
       </c>
     </row>
   </sheetData>
@@ -27745,6 +27745,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010003FE97044DB4FC4F901CA467E5223028" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a3f50da6d73106df175a7d9ecf5a4cc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="D77E192D-40C8-42D6-ACAD-759333CE872E" xmlns:ns3="d77e192d-40c8-42d6-acad-759333ce872e" xmlns:ns4="8df9d228-deee-4e36-845e-447b583fc1fe" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="72405369cf94f89852b763e35ae66afc" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="D77E192D-40C8-42D6-ACAD-759333CE872E"/>
@@ -27960,15 +27969,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C24D1664-4FDC-4778-99E5-9EDACEFF3E08}">
   <ds:schemaRefs>
@@ -27988,6 +27988,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3633D6CF-EA3A-4FA7-BECE-ED6AD27EBC88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{662A7507-D437-4535-ACBF-CE8183D0E8AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28005,12 +28013,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3633D6CF-EA3A-4FA7-BECE-ED6AD27EBC88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>